<commit_message>
add another time track template
</commit_message>
<xml_diff>
--- a/WorkSmarterNotHarder/controle-de-tempo.xlsx
+++ b/WorkSmarterNotHarder/controle-de-tempo.xlsx
@@ -9,9 +9,10 @@
   <sheets>
     <sheet name="Controle - 30 min" sheetId="1" r:id="rId1"/>
     <sheet name="Controle - 15 min" sheetId="2" r:id="rId2"/>
-    <sheet name="Reserva de Tempo" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Reserva de Tempo" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Registro de Atividades</t>
   </si>
@@ -49,12 +50,27 @@
   <si>
     <t>Dia</t>
   </si>
+  <si>
+    <t>Segunda</t>
+  </si>
+  <si>
+    <t>Terça</t>
+  </si>
+  <si>
+    <t>Quarta</t>
+  </si>
+  <si>
+    <t>Quinta</t>
+  </si>
+  <si>
+    <t>Sexta</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +107,12 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -106,7 +128,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -166,6 +188,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -174,24 +313,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="3" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -539,693 +699,698 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="34" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>0.25</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>0.27083333333333331</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>0.29166666666666702</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>0.3125</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>0.33333333333333298</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>0.375</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="5"/>
-      <c r="S12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>0.4375</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="5"/>
-      <c r="R13" s="5"/>
-      <c r="S13" s="5"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="5"/>
-      <c r="R14" s="5"/>
-      <c r="S14" s="5"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>0.47916666666666602</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>0.5</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="5"/>
-      <c r="S16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>0.52083333333333304</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="5"/>
-      <c r="S17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>0.54166666666666596</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="5"/>
-      <c r="R18" s="5"/>
-      <c r="S18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>0.5625</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>0.60416666666666596</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>0.625</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>0.64583333333333304</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="5"/>
-      <c r="R23" s="5"/>
-      <c r="S23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>0.66666666666666596</v>
       </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
-      <c r="P24" s="5"/>
-      <c r="Q24" s="5"/>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>0.6875</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="5"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>0.70833333333333304</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
-      <c r="P26" s="5"/>
-      <c r="Q26" s="5"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>0.72916666666666596</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>0.75</v>
       </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>0.77083333333333304</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>0.79166666666666663</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="R1:R3"/>
     <mergeCell ref="S1:S3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="I1:I3"/>
@@ -1240,11 +1405,6 @@
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="R1:R3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1259,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
@@ -1269,72 +1429,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
     </row>
     <row r="3" spans="1:19" ht="34" customHeight="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>0.25</v>
       </c>
       <c r="B4" s="1"/>
@@ -1357,7 +1517,7 @@
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>0.26041666666666669</v>
       </c>
       <c r="B5" s="1"/>
@@ -1380,7 +1540,7 @@
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>0.27083333333333298</v>
       </c>
       <c r="B6" s="1"/>
@@ -1403,7 +1563,7 @@
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>0.28125</v>
       </c>
       <c r="B7" s="1"/>
@@ -1426,7 +1586,7 @@
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>0.29166666666666702</v>
       </c>
       <c r="B8" s="1"/>
@@ -1449,7 +1609,7 @@
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>0.30208333333333298</v>
       </c>
       <c r="B9" s="1"/>
@@ -1472,7 +1632,7 @@
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>0.3125</v>
       </c>
       <c r="B10" s="1"/>
@@ -1495,7 +1655,7 @@
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>0.32291666666666702</v>
       </c>
       <c r="B11" s="1"/>
@@ -1518,7 +1678,7 @@
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>0.33333333333333298</v>
       </c>
       <c r="B12" s="1"/>
@@ -1541,7 +1701,7 @@
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>0.34375</v>
       </c>
       <c r="B13" s="1"/>
@@ -1564,7 +1724,7 @@
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>0.35416666666666702</v>
       </c>
       <c r="B14" s="1"/>
@@ -1587,7 +1747,7 @@
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>0.36458333333333398</v>
       </c>
       <c r="B15" s="1"/>
@@ -1610,7 +1770,7 @@
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>0.375</v>
       </c>
       <c r="B16" s="1"/>
@@ -1633,7 +1793,7 @@
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="3">
+      <c r="A17" s="2">
         <v>0.38541666666666702</v>
       </c>
       <c r="B17" s="1"/>
@@ -1656,7 +1816,7 @@
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>0.39583333333333398</v>
       </c>
       <c r="B18" s="1"/>
@@ -1679,7 +1839,7 @@
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="3">
+      <c r="A19" s="2">
         <v>0.40625</v>
       </c>
       <c r="B19" s="1"/>
@@ -1702,7 +1862,7 @@
       <c r="S19" s="1"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="3">
+      <c r="A20" s="2">
         <v>0.41666666666666702</v>
       </c>
       <c r="B20" s="1"/>
@@ -1725,7 +1885,7 @@
       <c r="S20" s="1"/>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="3">
+      <c r="A21" s="2">
         <v>0.42708333333333398</v>
       </c>
       <c r="B21" s="1"/>
@@ -1748,7 +1908,7 @@
       <c r="S21" s="1"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="3">
+      <c r="A22" s="2">
         <v>0.4375</v>
       </c>
       <c r="B22" s="1"/>
@@ -1771,7 +1931,7 @@
       <c r="S22" s="1"/>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="3">
+      <c r="A23" s="2">
         <v>0.44791666666666702</v>
       </c>
       <c r="B23" s="1"/>
@@ -1794,7 +1954,7 @@
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="3">
+      <c r="A24" s="2">
         <v>0.45833333333333398</v>
       </c>
       <c r="B24" s="1"/>
@@ -1817,7 +1977,7 @@
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19">
-      <c r="A25" s="3">
+      <c r="A25" s="2">
         <v>0.46875</v>
       </c>
       <c r="B25" s="1"/>
@@ -1840,7 +2000,7 @@
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="3">
+      <c r="A26" s="2">
         <v>0.47916666666666702</v>
       </c>
       <c r="B26" s="1"/>
@@ -1863,7 +2023,7 @@
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19">
-      <c r="A27" s="3">
+      <c r="A27" s="2">
         <v>0.48958333333333398</v>
       </c>
       <c r="B27" s="1"/>
@@ -1886,7 +2046,7 @@
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19">
-      <c r="A28" s="3">
+      <c r="A28" s="2">
         <v>0.5</v>
       </c>
       <c r="B28" s="1"/>
@@ -1909,7 +2069,7 @@
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="3">
+      <c r="A29" s="2">
         <v>0.51041666666666696</v>
       </c>
       <c r="B29" s="1"/>
@@ -1932,7 +2092,7 @@
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19">
-      <c r="A30" s="3">
+      <c r="A30" s="2">
         <v>0.52083333333333404</v>
       </c>
       <c r="B30" s="1"/>
@@ -1955,7 +2115,7 @@
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19">
-      <c r="A31" s="3">
+      <c r="A31" s="2">
         <v>0.53125</v>
       </c>
       <c r="B31" s="1"/>
@@ -1978,7 +2138,7 @@
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19">
-      <c r="A32" s="3">
+      <c r="A32" s="2">
         <v>0.54166666666666696</v>
       </c>
       <c r="B32" s="1"/>
@@ -2001,7 +2161,7 @@
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19">
-      <c r="A33" s="3">
+      <c r="A33" s="2">
         <v>0.55208333333333404</v>
       </c>
       <c r="B33" s="1"/>
@@ -2024,7 +2184,7 @@
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19">
-      <c r="A34" s="3">
+      <c r="A34" s="2">
         <v>0.562500000000001</v>
       </c>
       <c r="B34" s="1"/>
@@ -2047,7 +2207,7 @@
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="A35" s="3">
+      <c r="A35" s="2">
         <v>0.57291666666666696</v>
       </c>
       <c r="B35" s="1"/>
@@ -2070,7 +2230,7 @@
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19">
-      <c r="A36" s="3">
+      <c r="A36" s="2">
         <v>0.58333333333333404</v>
       </c>
       <c r="B36" s="1"/>
@@ -2093,7 +2253,7 @@
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="3">
+      <c r="A37" s="2">
         <v>0.593750000000001</v>
       </c>
       <c r="B37" s="1"/>
@@ -2116,7 +2276,7 @@
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19">
-      <c r="A38" s="3">
+      <c r="A38" s="2">
         <v>0.60416666666666696</v>
       </c>
       <c r="B38" s="1"/>
@@ -2139,7 +2299,7 @@
       <c r="S38" s="1"/>
     </row>
     <row r="39" spans="1:19">
-      <c r="A39" s="3">
+      <c r="A39" s="2">
         <v>0.61458333333333404</v>
       </c>
       <c r="B39" s="1"/>
@@ -2162,7 +2322,7 @@
       <c r="S39" s="1"/>
     </row>
     <row r="40" spans="1:19">
-      <c r="A40" s="3">
+      <c r="A40" s="2">
         <v>0.625000000000001</v>
       </c>
       <c r="B40" s="1"/>
@@ -2185,7 +2345,7 @@
       <c r="S40" s="1"/>
     </row>
     <row r="41" spans="1:19">
-      <c r="A41" s="3">
+      <c r="A41" s="2">
         <v>0.63541666666666696</v>
       </c>
       <c r="B41" s="1"/>
@@ -2208,7 +2368,7 @@
       <c r="S41" s="1"/>
     </row>
     <row r="42" spans="1:19">
-      <c r="A42" s="3">
+      <c r="A42" s="2">
         <v>0.64583333333333404</v>
       </c>
       <c r="B42" s="1"/>
@@ -2231,7 +2391,7 @@
       <c r="S42" s="1"/>
     </row>
     <row r="43" spans="1:19">
-      <c r="A43" s="3">
+      <c r="A43" s="2">
         <v>0.656250000000001</v>
       </c>
       <c r="B43" s="1"/>
@@ -2254,7 +2414,7 @@
       <c r="S43" s="1"/>
     </row>
     <row r="44" spans="1:19">
-      <c r="A44" s="3">
+      <c r="A44" s="2">
         <v>0.66666666666666696</v>
       </c>
       <c r="B44" s="1"/>
@@ -2277,7 +2437,7 @@
       <c r="S44" s="1"/>
     </row>
     <row r="45" spans="1:19">
-      <c r="A45" s="3">
+      <c r="A45" s="2">
         <v>0.67708333333333404</v>
       </c>
       <c r="B45" s="1"/>
@@ -2300,7 +2460,7 @@
       <c r="S45" s="1"/>
     </row>
     <row r="46" spans="1:19">
-      <c r="A46" s="3">
+      <c r="A46" s="2">
         <v>0.687500000000001</v>
       </c>
       <c r="B46" s="1"/>
@@ -2323,7 +2483,7 @@
       <c r="S46" s="1"/>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" s="3">
+      <c r="A47" s="2">
         <v>0.69791666666666696</v>
       </c>
       <c r="B47" s="1"/>
@@ -2346,7 +2506,7 @@
       <c r="S47" s="1"/>
     </row>
     <row r="48" spans="1:19">
-      <c r="A48" s="3">
+      <c r="A48" s="2">
         <v>0.70833333333333404</v>
       </c>
       <c r="B48" s="1"/>
@@ -2369,7 +2529,7 @@
       <c r="S48" s="1"/>
     </row>
     <row r="49" spans="1:19">
-      <c r="A49" s="3">
+      <c r="A49" s="2">
         <v>0.718750000000001</v>
       </c>
       <c r="B49" s="1"/>
@@ -2392,7 +2552,7 @@
       <c r="S49" s="1"/>
     </row>
     <row r="50" spans="1:19">
-      <c r="A50" s="3">
+      <c r="A50" s="2">
         <v>0.72916666666666796</v>
       </c>
       <c r="B50" s="1"/>
@@ -2415,7 +2575,7 @@
       <c r="S50" s="1"/>
     </row>
     <row r="51" spans="1:19">
-      <c r="A51" s="3">
+      <c r="A51" s="2">
         <v>0.73958333333333404</v>
       </c>
       <c r="B51" s="1"/>
@@ -2438,7 +2598,7 @@
       <c r="S51" s="1"/>
     </row>
     <row r="52" spans="1:19">
-      <c r="A52" s="3">
+      <c r="A52" s="2">
         <v>0.750000000000001</v>
       </c>
       <c r="B52" s="1"/>
@@ -2461,7 +2621,7 @@
       <c r="S52" s="1"/>
     </row>
     <row r="53" spans="1:19">
-      <c r="A53" s="3">
+      <c r="A53" s="2">
         <v>0.76041666666666796</v>
       </c>
       <c r="B53" s="1"/>
@@ -2484,7 +2644,7 @@
       <c r="S53" s="1"/>
     </row>
     <row r="54" spans="1:19">
-      <c r="A54" s="3">
+      <c r="A54" s="2">
         <v>0.77083333333333404</v>
       </c>
       <c r="B54" s="1"/>
@@ -2507,7 +2667,7 @@
       <c r="S54" s="1"/>
     </row>
     <row r="55" spans="1:19">
-      <c r="A55" s="3">
+      <c r="A55" s="2">
         <v>0.781250000000001</v>
       </c>
       <c r="B55" s="1"/>
@@ -2530,7 +2690,7 @@
       <c r="S55" s="1"/>
     </row>
     <row r="56" spans="1:19">
-      <c r="A56" s="3">
+      <c r="A56" s="2">
         <v>0.79166666666666796</v>
       </c>
       <c r="B56" s="1"/>
@@ -2554,6 +2714,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="S1:S3"/>
+    <mergeCell ref="M1:M3"/>
+    <mergeCell ref="N1:N3"/>
+    <mergeCell ref="O1:O3"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="R1:R3"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
@@ -2566,13 +2733,6 @@
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="K1:K3"/>
-    <mergeCell ref="S1:S3"/>
-    <mergeCell ref="M1:M3"/>
-    <mergeCell ref="N1:N3"/>
-    <mergeCell ref="O1:O3"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="R1:R3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2585,9 +2745,584 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="23">
+      <c r="B2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+    </row>
+    <row r="3" spans="2:7" ht="23">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="B4" s="21">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="22">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="22">
+        <v>0.3125</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="23">
+        <v>0.32291666666666702</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="21">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="22">
+        <v>0.34375</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="22">
+        <v>0.35416666666666602</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="23">
+        <v>0.36458333333333298</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="21">
+        <v>0.375</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="22">
+        <v>0.38541666666666602</v>
+      </c>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="22">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="23">
+        <v>0.40625</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="21">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="22">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="22">
+        <v>0.4375</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="23">
+        <v>0.44791666666666602</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="21">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="22">
+        <v>0.46875</v>
+      </c>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="22">
+        <v>0.47916666666666602</v>
+      </c>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="23">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="16"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="22">
+        <v>0.51041666666666596</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="22">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="23">
+        <v>0.531249999999999</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="21">
+        <v>0.54166666666666596</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="22">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="22">
+        <v>0.562499999999999</v>
+      </c>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="23">
+        <v>0.57291666666666596</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="21">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="22">
+        <v>0.593749999999999</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="22">
+        <v>0.60416666666666596</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="23">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="16"/>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="21">
+        <v>0.624999999999999</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="12"/>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="22">
+        <v>0.63541666666666596</v>
+      </c>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="14"/>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="22">
+        <v>0.64583333333333204</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="14"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="23">
+        <v>0.656249999999999</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="16"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="21">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="22">
+        <v>0.67708333333333204</v>
+      </c>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="14"/>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="22">
+        <v>0.687499999999999</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="14"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="23">
+        <v>0.69791666666666596</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="16"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="21">
+        <v>0.70833333333333204</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="12"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="22">
+        <v>0.718749999999999</v>
+      </c>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="14"/>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="22">
+        <v>0.72916666666666496</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="14"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="23">
+        <v>0.73958333333333204</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="16"/>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" s="21">
+        <v>0.749999999999999</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="12"/>
+    </row>
+    <row r="49" spans="2:7">
+      <c r="B49" s="22">
+        <v>0.76041666666666496</v>
+      </c>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="2:7">
+      <c r="B50" s="22">
+        <v>0.77083333333333204</v>
+      </c>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="2:7">
+      <c r="B51" s="22">
+        <v>0.781249999999999</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="2:7">
+      <c r="B52" s="21">
+        <v>0.79166666666666496</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="12"/>
+    </row>
+    <row r="53" spans="2:7">
+      <c r="B53" s="22">
+        <v>0.80208333333332904</v>
+      </c>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="14"/>
+    </row>
+    <row r="54" spans="2:7">
+      <c r="B54" s="22">
+        <v>0.812499999999995</v>
+      </c>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="14"/>
+    </row>
+    <row r="55" spans="2:7">
+      <c r="B55" s="23">
+        <v>0.82291666666666097</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
+      <c r="E55" s="15"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2598,25 +3333,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="4">
         <v>0</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="4">
         <f>C2-C30</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2627,10 +3362,10 @@
     <row r="6" spans="2:6">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="4">
         <f>30*24</f>
         <v>720</v>
       </c>
@@ -2638,10 +3373,10 @@
     <row r="7" spans="2:6">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="4">
         <f>7*24</f>
         <v>168</v>
       </c>
@@ -2649,10 +3384,10 @@
     <row r="8" spans="2:6">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="4">
         <f>24*1</f>
         <v>24</v>
       </c>
@@ -2742,10 +3477,10 @@
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="2:3">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="4">
         <f>SUM(C5:C29)</f>
         <v>0</v>
       </c>

</xml_diff>